<commit_message>
a few new plots. mid-statsModels run
</commit_message>
<xml_diff>
--- a/dataIn/interactionTable.xlsx
+++ b/dataIn/interactionTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
   <si>
     <t xml:space="preserve">  airTemp</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sweLS</t>
+  </si>
+  <si>
+    <t>prcpLS</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -166,9 +172,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -493,12 +496,12 @@
   <dimension ref="A2:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="19" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -549,124 +552,126 @@
         <v>14</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="S2" s="10"/>
       <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="11"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="11"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="12"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="12"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="12"/>
@@ -674,21 +679,21 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="12"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
     </row>
     <row r="9" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -703,20 +708,20 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="12"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
     </row>
     <row r="10" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -732,19 +737,19 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="12"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
     </row>
     <row r="11" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="12"/>
@@ -755,18 +760,18 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="12"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="13"/>
@@ -780,17 +785,17 @@
       <c r="J12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="13"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="13"/>
@@ -803,16 +808,16 @@
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="13"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -832,15 +837,15 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="13"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -865,14 +870,14 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="13"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
     </row>
     <row r="16" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="14"/>
@@ -898,13 +903,13 @@
       <c r="N16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="14"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
     </row>
     <row r="17" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="14"/>
@@ -931,12 +936,12 @@
         <v>16</v>
       </c>
       <c r="O17" s="14"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="14"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -966,26 +971,31 @@
       <c r="P18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="14"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
       <c r="R19" s="15"/>
     </row>
   </sheetData>

</xml_diff>